<commit_message>
add thêm ví dụ
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12495" activeTab="1"/>
+    <workbookView windowWidth="28125" windowHeight="12495" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="5 nguyên ly solid" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,16 @@
     <sheet name="@Restcontroller" sheetId="4" r:id="rId4"/>
     <sheet name="@Scope" sheetId="5" r:id="rId5"/>
     <sheet name="@Configuration &amp; @Bean" sheetId="6" r:id="rId6"/>
+    <sheet name="CORS" sheetId="7" r:id="rId7"/>
+    <sheet name="Sheet2" sheetId="8" r:id="rId8"/>
+    <sheet name="Sheet3" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
   <si>
     <t>Single responsibility priciple</t>
   </si>
@@ -83,7 +86,7 @@
     <t>DI</t>
   </si>
   <si>
-    <t>IoC là viết tắt của Inversion of Control, hay còn gọi là Dependency Injection (DI). IoC là một nguyên tắc thiết kế phần mềm, trong đó vai trò điều khiển luồng của chương trình được đảo ngược hoàn toàn.
+    <t>IoC là viết tắt của Inversion of Control. IoC là một nguyên tắc thiết kế phần mềm, trong đó vai trò điều khiển luồng của chương trình được đảo ngược hoàn toàn.
 Trong truyền thống, các đối tượng có thể được tạo và sử dụng bằng cách khởi tạo chúng bên trong lớp hoặc đối tượng khác. Khi sử dụng IoC, các đối tượng không được tạo bên trong lớp hoặc đối tượng đó, mà được tạo và quản lý bởi một bên thứ ba, thường là một container, chẳng hạn như Spring IoC container.</t>
   </si>
   <si>
@@ -111,7 +114,7 @@
     <t>Restcontroller</t>
   </si>
   <si>
-    <t>Service</t>
+    <t>@Service</t>
   </si>
   <si>
     <t>Repository</t>
@@ -154,25 +157,49 @@
   <si>
     <t>Trong Spring Core, @Bean là một annotation được sử dụng để đánh dấu một phương thức trả về đối tượng nào đó là một bean. Bean là một đối tượng được quản lý bởi Spring IoC container và được sử dụng trong ứng dụng.</t>
   </si>
+  <si>
+    <t>CORS</t>
+  </si>
+  <si>
+    <t>CORS là một cơ chế cho phép nhiều tài nguyên khác nhau (fonts, Javascript, v.v…) của một trang web có thể được truy vấn từ domain khác với domain của trang đó. CORS là viết tắt của từ Cross-origin resource sharing
+Khi call API tới server mà không có header Access-Control-Allow-Origin hoặc giá trị của nó không hợp lệ thì sẽ phát sinh lỗi này và không lấy được dữ liệu từ API. Cách khắc phục lỗi trên là phải config enable CORS lên để phía client có thể gọi được dữ liệu</t>
+  </si>
+  <si>
+    <t>Ngăn chặn việc truy cập tài nguyên của các domain khác một cách vô tội vạ.
+Chia sẻ tài nguyên giữa các trang web khác miền nhau.
+Cho phép các ứng dụng web chạy trên các tên miền khác nhau truy cập tài nguyên trên máy chủ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SOLID Principles(5 nguyên tắc thiết kế): mỗi nguyên tắc cho một ví dụ
+2. Inversion of Control
+3. Dependency Injection
+4. Tìm hiểu về Spring Core
+ - Tìm hiểu về các component(thành phần) của spring core
+  +  Spring Component: các annotation @RestController, @Service, @Repository
+  +  annotation @Scope
+  +  annotation @Configuration, @Bean: using for IOC Container</t>
+  </si>
+  <si>
+    <t>1 cho thấy sự phụ thuộc</t>
+  </si>
+  <si>
+    <t>2 các cách triển khai cors</t>
+  </si>
+  <si>
+    <t>3 loại bỏ sự phụ thuộc bằng interface</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="22">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,10 +222,26 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -209,9 +252,39 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -226,30 +299,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -258,22 +307,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -287,8 +321,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -303,7 +338,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -311,22 +353,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -347,7 +374,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -359,7 +422,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -371,13 +446,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -389,37 +518,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -431,97 +548,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -532,6 +559,30 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -546,32 +597,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -600,6 +625,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -609,26 +649,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -637,7 +664,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -655,130 +682,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -789,25 +816,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1499,7 +1526,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1057275" y="4900930"/>
+          <a:off x="1057275" y="4710430"/>
           <a:ext cx="5556885" cy="4630420"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1516,13 +1543,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1057275</xdr:colOff>
+      <xdr:colOff>1047750</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>300990</xdr:colOff>
+      <xdr:colOff>291465</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>86995</xdr:rowOff>
     </xdr:to>
@@ -1541,7 +1568,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7400925" y="4445000"/>
+          <a:off x="7391400" y="4254500"/>
           <a:ext cx="7769860" cy="4201795"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1582,7 +1609,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="600075" y="2057400"/>
+          <a:off x="600075" y="2476500"/>
           <a:ext cx="304800" cy="312420"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1834,7 +1861,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13786485" y="2438400"/>
+          <a:off x="13786485" y="2857500"/>
           <a:ext cx="304800" cy="312420"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1876,7 +1903,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10586085" y="2247900"/>
+          <a:off x="10586085" y="2667000"/>
           <a:ext cx="304800" cy="312420"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1918,7 +1945,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10586085" y="2247900"/>
+          <a:off x="10586085" y="2667000"/>
           <a:ext cx="304800" cy="312420"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1960,7 +1987,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10586085" y="2247900"/>
+          <a:off x="10586085" y="2667000"/>
           <a:ext cx="304800" cy="312420"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2002,7 +2029,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10586085" y="2247900"/>
+          <a:off x="10586085" y="2667000"/>
           <a:ext cx="304800" cy="312420"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2044,7 +2071,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10586085" y="2247900"/>
+          <a:off x="10586085" y="2667000"/>
           <a:ext cx="304800" cy="312420"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2086,7 +2113,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10586085" y="2247900"/>
+          <a:off x="10586085" y="2667000"/>
           <a:ext cx="304800" cy="312420"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2128,7 +2155,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10586085" y="2247900"/>
+          <a:off x="10586085" y="2667000"/>
           <a:ext cx="304800" cy="312420"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2170,7 +2197,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10586085" y="2247900"/>
+          <a:off x="10586085" y="2667000"/>
           <a:ext cx="304800" cy="312420"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2218,7 +2245,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="645795" y="2209800"/>
+          <a:off x="645795" y="2628900"/>
           <a:ext cx="5280660" cy="2644140"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2284,6 +2311,53 @@
             </a14:hiddenFill>
           </a:ext>
         </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>48895</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>538480</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>92075</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="How do Cross Origin Resource Sharing (CORS) Headers work?"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1" r:link="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6819900" y="48895"/>
+          <a:ext cx="9996805" cy="5377180"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -2551,8 +2625,8 @@
   <sheetPr/>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1047619047619" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="5"/>
@@ -2635,7 +2709,7 @@
   <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+    <sheetView topLeftCell="A94" workbookViewId="0">
       <selection activeCell="P150" sqref="P150"/>
     </sheetView>
   </sheetViews>
@@ -2653,7 +2727,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1047619047619" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="2"/>
@@ -2671,14 +2745,14 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" ht="105" spans="1:3">
+    <row r="2" ht="90" spans="1:3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2686,19 +2760,19 @@
       <c r="A3" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="6"/>
+      <c r="C3" s="5"/>
     </row>
     <row r="4" ht="65" customHeight="1" spans="1:3">
       <c r="A4" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="6"/>
+      <c r="C4" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2717,7 +2791,7 @@
   <dimension ref="B1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="3"/>
@@ -2734,18 +2808,18 @@
       <c r="C1" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" ht="147" customHeight="1" spans="2:4">
-      <c r="B2" s="4" t="s">
+    <row r="2" ht="180" spans="2:4">
+      <c r="B2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>30</v>
       </c>
     </row>
@@ -2763,7 +2837,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="1"/>
@@ -2773,20 +2847,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:2">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2" ht="90" spans="1:2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="3" ht="225" spans="2:2">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2803,7 +2877,7 @@
   <dimension ref="B1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2"/>
@@ -2821,11 +2895,111 @@
       </c>
     </row>
     <row r="2" ht="60" spans="2:3">
+      <c r="B2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="10.4285714285714" customWidth="1"/>
+    <col min="2" max="2" width="87.4285714285714" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:2">
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" ht="90" spans="1:2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
       <c r="B2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" ht="45" spans="1:2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="64.2857142857143" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="135" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>